<commit_message>
kafka test jmx port
</commit_message>
<xml_diff>
--- a/docs/设计资料/bigdata-platform-architect.xlsx
+++ b/docs/设计资料/bigdata-platform-architect.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wujiulin/workspace/deployment/docs/设计资料/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baozhiwang/local_dir/codes/deployment/docs/设计资料/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="24760" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="24760" windowHeight="15540" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="应用规划" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="迁移执行计划事宜" sheetId="6" r:id="rId7"/>
     <sheet name="模拟迁移" sheetId="7" r:id="rId8"/>
     <sheet name="模拟迁移立项排期" sheetId="8" r:id="rId9"/>
+    <sheet name="测试环境" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -996,7 +997,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3518" uniqueCount="1439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3523" uniqueCount="1443">
   <si>
     <t>YARN</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1363,6 +1364,7 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>业务线作业</t>
@@ -1382,6 +1384,7 @@
         <color theme="1"/>
         <rFont val="宋体"/>
         <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>/虎鲸业务线BI作业</t>
@@ -10738,6 +10741,33 @@
   </si>
   <si>
     <t>20390</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务</t>
+    <rPh sb="0" eb="1">
+      <t>fu wu</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kafka3 JMX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器</t>
+    <rPh sb="0" eb="1">
+      <t>ji qi</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigtest-appsvr-129-1
+bigtest-appsvr-129-2
+bigtest-appsvr-129-3
+bigtest-appsvr-129-4
+bigtest-appsvr-129-5
+bigtest-appsvr-129-6</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -10751,6 +10781,7 @@
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11279,7 +11310,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -11611,6 +11642,9 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11624,10 +11658,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -11641,8 +11675,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="167">
@@ -12184,7 +12218,7 @@
       <c r="Y1" s="21"/>
     </row>
     <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.15">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="138" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="118" t="s">
@@ -12231,7 +12265,7 @@
       <c r="Y2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="45" x14ac:dyDescent="0.15">
-      <c r="A3" s="137"/>
+      <c r="A3" s="138"/>
       <c r="B3" s="118" t="s">
         <v>8</v>
       </c>
@@ -12278,7 +12312,7 @@
       <c r="Y3" s="18"/>
     </row>
     <row r="4" spans="1:26" ht="45" x14ac:dyDescent="0.15">
-      <c r="A4" s="137"/>
+      <c r="A4" s="138"/>
       <c r="B4" s="118" t="s">
         <v>9</v>
       </c>
@@ -12331,7 +12365,7 @@
       <c r="Y4" s="18"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="138" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="118" t="s">
@@ -12380,7 +12414,7 @@
       <c r="Y5" s="18"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A6" s="137"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="118" t="s">
         <v>362</v>
       </c>
@@ -12427,7 +12461,7 @@
       <c r="Y6" s="18"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A7" s="137"/>
+      <c r="A7" s="138"/>
       <c r="B7" s="118" t="s">
         <v>531</v>
       </c>
@@ -12474,7 +12508,7 @@
       <c r="Y7" s="18"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A8" s="137"/>
+      <c r="A8" s="138"/>
       <c r="B8" s="118" t="s">
         <v>532</v>
       </c>
@@ -12521,7 +12555,7 @@
       <c r="Y8" s="18"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A9" s="137"/>
+      <c r="A9" s="138"/>
       <c r="B9" s="118" t="s">
         <v>533</v>
       </c>
@@ -12648,7 +12682,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.15">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="138" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="118" t="s">
@@ -12706,7 +12740,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A12" s="137"/>
+      <c r="A12" s="138"/>
       <c r="B12" s="118" t="s">
         <v>535</v>
       </c>
@@ -12762,7 +12796,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.15">
-      <c r="A13" s="137"/>
+      <c r="A13" s="138"/>
       <c r="B13" s="118" t="s">
         <v>363</v>
       </c>
@@ -12818,7 +12852,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.15">
-      <c r="A14" s="137"/>
+      <c r="A14" s="138"/>
       <c r="B14" s="118" t="s">
         <v>364</v>
       </c>
@@ -12871,7 +12905,7 @@
       <c r="Y14" s="18"/>
     </row>
     <row r="15" spans="1:26" ht="60" x14ac:dyDescent="0.15">
-      <c r="A15" s="137"/>
+      <c r="A15" s="138"/>
       <c r="B15" s="118" t="s">
         <v>365</v>
       </c>
@@ -12924,7 +12958,7 @@
       <c r="Y15" s="18"/>
     </row>
     <row r="16" spans="1:26" ht="45" x14ac:dyDescent="0.15">
-      <c r="A16" s="137"/>
+      <c r="A16" s="138"/>
       <c r="B16" s="118" t="s">
         <v>366</v>
       </c>
@@ -12977,7 +13011,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" ht="45" x14ac:dyDescent="0.15">
-      <c r="A17" s="137"/>
+      <c r="A17" s="138"/>
       <c r="B17" s="118" t="s">
         <v>367</v>
       </c>
@@ -13083,7 +13117,7 @@
       <c r="Y18" s="21"/>
     </row>
     <row r="19" spans="1:25" ht="45" x14ac:dyDescent="0.15">
-      <c r="A19" s="137" t="s">
+      <c r="A19" s="138" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="118" t="s">
@@ -13120,7 +13154,7 @@
       <c r="Y19" s="18"/>
     </row>
     <row r="20" spans="1:25" ht="45" x14ac:dyDescent="0.15">
-      <c r="A20" s="137"/>
+      <c r="A20" s="138"/>
       <c r="B20" s="118" t="s">
         <v>28</v>
       </c>
@@ -13155,7 +13189,7 @@
       <c r="Y20" s="18"/>
     </row>
     <row r="21" spans="1:25" ht="45" x14ac:dyDescent="0.15">
-      <c r="A21" s="137"/>
+      <c r="A21" s="138"/>
       <c r="B21" s="118" t="s">
         <v>29</v>
       </c>
@@ -13190,7 +13224,7 @@
       <c r="Y21" s="18"/>
     </row>
     <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.15">
-      <c r="A22" s="137"/>
+      <c r="A22" s="138"/>
       <c r="B22" s="118" t="s">
         <v>30</v>
       </c>
@@ -13225,7 +13259,7 @@
       <c r="Y22" s="18"/>
     </row>
     <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.15">
-      <c r="A23" s="137"/>
+      <c r="A23" s="138"/>
       <c r="B23" s="118" t="s">
         <v>31</v>
       </c>
@@ -13260,7 +13294,7 @@
       <c r="Y23" s="18"/>
     </row>
     <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.15">
-      <c r="A24" s="137"/>
+      <c r="A24" s="138"/>
       <c r="B24" s="118" t="s">
         <v>34</v>
       </c>
@@ -13301,7 +13335,7 @@
       <c r="Y24" s="18"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A25" s="137"/>
+      <c r="A25" s="138"/>
       <c r="B25" s="118" t="s">
         <v>36</v>
       </c>
@@ -13340,7 +13374,7 @@
       <c r="Y25" s="18"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A26" s="137"/>
+      <c r="A26" s="138"/>
       <c r="B26" s="118" t="s">
         <v>37</v>
       </c>
@@ -13379,7 +13413,7 @@
       <c r="Y26" s="18"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A27" s="137"/>
+      <c r="A27" s="138"/>
       <c r="B27" s="118" t="s">
         <v>38</v>
       </c>
@@ -13414,7 +13448,7 @@
       <c r="Y27" s="18"/>
     </row>
     <row r="28" spans="1:25" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="137"/>
+      <c r="A28" s="138"/>
       <c r="B28" s="118" t="s">
         <v>42</v>
       </c>
@@ -13449,7 +13483,7 @@
       <c r="Y28" s="18"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A29" s="137"/>
+      <c r="A29" s="138"/>
       <c r="B29" s="118" t="s">
         <v>163</v>
       </c>
@@ -13484,7 +13518,7 @@
       <c r="Y29" s="18"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A30" s="137"/>
+      <c r="A30" s="138"/>
       <c r="B30" s="118" t="s">
         <v>310</v>
       </c>
@@ -13519,7 +13553,7 @@
       <c r="Y30" s="18"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A31" s="137"/>
+      <c r="A31" s="138"/>
       <c r="B31" s="118" t="s">
         <v>311</v>
       </c>
@@ -13554,7 +13588,7 @@
       <c r="Y31" s="18"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A32" s="137"/>
+      <c r="A32" s="138"/>
       <c r="B32" s="118" t="s">
         <v>312</v>
       </c>
@@ -13636,11 +13670,54 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B2">
+        <v>19094</v>
+      </c>
+      <c r="C2" s="148" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -18158,7 +18235,7 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A98" s="147"/>
+      <c r="A98" s="137"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E99" s="1" t="s">
@@ -19638,7 +19715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="102" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -20089,13 +20166,13 @@
       <c r="A41" s="123" t="s">
         <v>1327</v>
       </c>
-      <c r="B41" s="139" t="s">
+      <c r="B41" s="140" t="s">
         <v>1329</v>
       </c>
       <c r="C41" s="119"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
-      <c r="F41" s="138" t="s">
+      <c r="F41" s="139" t="s">
         <v>1320</v>
       </c>
     </row>
@@ -20103,227 +20180,227 @@
       <c r="A42" s="123" t="s">
         <v>1262</v>
       </c>
-      <c r="B42" s="139"/>
+      <c r="B42" s="140"/>
       <c r="C42" s="119"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="138"/>
+      <c r="F42" s="139"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="123" t="s">
         <v>1263</v>
       </c>
-      <c r="B43" s="139"/>
+      <c r="B43" s="140"/>
       <c r="C43" s="119"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
-      <c r="F43" s="138"/>
+      <c r="F43" s="139"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="123" t="s">
         <v>1335</v>
       </c>
-      <c r="B44" s="139"/>
+      <c r="B44" s="140"/>
       <c r="C44" s="119"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
-      <c r="F44" s="138"/>
+      <c r="F44" s="139"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="123" t="s">
         <v>1303</v>
       </c>
-      <c r="B45" s="139"/>
+      <c r="B45" s="140"/>
       <c r="C45" s="119"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
-      <c r="F45" s="138"/>
+      <c r="F45" s="139"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="123" t="s">
         <v>1311</v>
       </c>
-      <c r="B46" s="139"/>
+      <c r="B46" s="140"/>
       <c r="C46" s="119"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
-      <c r="F46" s="138"/>
+      <c r="F46" s="139"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="124" t="s">
         <v>1336</v>
       </c>
-      <c r="B47" s="139"/>
+      <c r="B47" s="140"/>
       <c r="C47" s="119"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
-      <c r="F47" s="138"/>
+      <c r="F47" s="139"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="124" t="s">
         <v>1305</v>
       </c>
-      <c r="B48" s="139"/>
+      <c r="B48" s="140"/>
       <c r="C48" s="119"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
-      <c r="F48" s="138"/>
+      <c r="F48" s="139"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="124" t="s">
         <v>1313</v>
       </c>
-      <c r="B49" s="139"/>
+      <c r="B49" s="140"/>
       <c r="C49" s="119"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="138"/>
+      <c r="F49" s="139"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="124" t="s">
         <v>1318</v>
       </c>
-      <c r="B50" s="139"/>
+      <c r="B50" s="140"/>
       <c r="C50" s="119"/>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
-      <c r="F50" s="138"/>
+      <c r="F50" s="139"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="124" t="s">
         <v>1291</v>
       </c>
-      <c r="B51" s="139"/>
+      <c r="B51" s="140"/>
       <c r="C51" s="119"/>
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
-      <c r="F51" s="138"/>
+      <c r="F51" s="139"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="124" t="s">
         <v>1306</v>
       </c>
-      <c r="B52" s="139"/>
+      <c r="B52" s="140"/>
       <c r="C52" s="119"/>
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
-      <c r="F52" s="138"/>
+      <c r="F52" s="139"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="124" t="s">
         <v>1314</v>
       </c>
-      <c r="B53" s="139"/>
+      <c r="B53" s="140"/>
       <c r="C53" s="119"/>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
-      <c r="F53" s="138"/>
+      <c r="F53" s="139"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="124" t="s">
         <v>1295</v>
       </c>
-      <c r="B54" s="139"/>
+      <c r="B54" s="140"/>
       <c r="C54" s="119"/>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
-      <c r="F54" s="138"/>
+      <c r="F54" s="139"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="124" t="s">
         <v>1307</v>
       </c>
-      <c r="B55" s="139"/>
+      <c r="B55" s="140"/>
       <c r="C55" s="119"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
-      <c r="F55" s="138"/>
+      <c r="F55" s="139"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="124" t="s">
         <v>1315</v>
       </c>
-      <c r="B56" s="139"/>
+      <c r="B56" s="140"/>
       <c r="C56" s="119"/>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
-      <c r="F56" s="138"/>
+      <c r="F56" s="139"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="139"/>
+      <c r="B57" s="140"/>
       <c r="C57" s="119"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
-      <c r="F57" s="138"/>
+      <c r="F57" s="139"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="124" t="s">
         <v>1265</v>
       </c>
-      <c r="B58" s="139"/>
+      <c r="B58" s="140"/>
       <c r="C58" s="119"/>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
-      <c r="F58" s="138"/>
+      <c r="F58" s="139"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="124" t="s">
         <v>1298</v>
       </c>
-      <c r="B59" s="139"/>
+      <c r="B59" s="140"/>
       <c r="C59" s="119"/>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="138"/>
+      <c r="F59" s="139"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="124" t="s">
         <v>1316</v>
       </c>
-      <c r="B60" s="139"/>
+      <c r="B60" s="140"/>
       <c r="C60" s="119"/>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
-      <c r="F60" s="138"/>
+      <c r="F60" s="139"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="124" t="s">
         <v>1266</v>
       </c>
-      <c r="B61" s="139"/>
+      <c r="B61" s="140"/>
       <c r="C61" s="119"/>
       <c r="D61" s="17"/>
       <c r="E61" s="17"/>
-      <c r="F61" s="138"/>
+      <c r="F61" s="139"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="124" t="s">
         <v>1301</v>
       </c>
-      <c r="B62" s="139"/>
+      <c r="B62" s="140"/>
       <c r="C62" s="119"/>
       <c r="D62" s="17"/>
       <c r="E62" s="17"/>
-      <c r="F62" s="138"/>
+      <c r="F62" s="139"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="124" t="s">
         <v>1310</v>
       </c>
-      <c r="B63" s="139"/>
+      <c r="B63" s="140"/>
       <c r="C63" s="119"/>
       <c r="D63" s="17"/>
       <c r="E63" s="17"/>
-      <c r="F63" s="138"/>
+      <c r="F63" s="139"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="124" t="s">
         <v>80</v>
       </c>
-      <c r="B64" s="139"/>
+      <c r="B64" s="140"/>
       <c r="C64" s="119"/>
       <c r="D64" s="17"/>
       <c r="E64" s="17"/>
@@ -20349,13 +20426,13 @@
       <c r="A66" s="125" t="s">
         <v>1278</v>
       </c>
-      <c r="B66" s="140" t="s">
+      <c r="B66" s="141" t="s">
         <v>1330</v>
       </c>
       <c r="C66" s="119"/>
       <c r="D66" s="17"/>
       <c r="E66" s="17"/>
-      <c r="F66" s="138" t="s">
+      <c r="F66" s="139" t="s">
         <v>1321</v>
       </c>
     </row>
@@ -20363,71 +20440,71 @@
       <c r="A67" s="125" t="s">
         <v>1286</v>
       </c>
-      <c r="B67" s="140"/>
+      <c r="B67" s="141"/>
       <c r="C67" s="119"/>
       <c r="D67" s="17"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="138"/>
+      <c r="F67" s="139"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="125" t="s">
         <v>1274</v>
       </c>
-      <c r="B68" s="140"/>
+      <c r="B68" s="141"/>
       <c r="C68" s="119"/>
       <c r="D68" s="17"/>
       <c r="E68" s="17"/>
-      <c r="F68" s="138"/>
+      <c r="F68" s="139"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="125" t="s">
         <v>1299</v>
       </c>
-      <c r="B69" s="140"/>
+      <c r="B69" s="141"/>
       <c r="C69" s="119"/>
       <c r="D69" s="17"/>
       <c r="E69" s="17"/>
-      <c r="F69" s="138"/>
+      <c r="F69" s="139"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="125" t="s">
         <v>1308</v>
       </c>
-      <c r="B70" s="140"/>
+      <c r="B70" s="141"/>
       <c r="C70" s="119"/>
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
-      <c r="F70" s="138"/>
+      <c r="F70" s="139"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="125" t="s">
         <v>1302</v>
       </c>
-      <c r="B71" s="140"/>
+      <c r="B71" s="141"/>
       <c r="C71" s="119"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
-      <c r="F71" s="138"/>
+      <c r="F71" s="139"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="140"/>
+      <c r="B72" s="141"/>
       <c r="C72" s="119"/>
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
-      <c r="F72" s="138"/>
+      <c r="F72" s="139"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="125" t="s">
         <v>1292</v>
       </c>
-      <c r="B73" s="140"/>
+      <c r="B73" s="141"/>
       <c r="C73" s="119"/>
       <c r="D73" s="17"/>
       <c r="E73" s="17"/>
-      <c r="F73" s="138" t="s">
+      <c r="F73" s="139" t="s">
         <v>1323</v>
       </c>
     </row>
@@ -20435,57 +20512,57 @@
       <c r="A74" s="125" t="s">
         <v>1268</v>
       </c>
-      <c r="B74" s="140"/>
+      <c r="B74" s="141"/>
       <c r="C74" s="119"/>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
-      <c r="F74" s="138"/>
+      <c r="F74" s="139"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="125" t="s">
         <v>1300</v>
       </c>
-      <c r="B75" s="140"/>
+      <c r="B75" s="141"/>
       <c r="C75" s="119"/>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
-      <c r="F75" s="138"/>
+      <c r="F75" s="139"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="125" t="s">
         <v>1304</v>
       </c>
-      <c r="B76" s="140"/>
+      <c r="B76" s="141"/>
       <c r="C76" s="119"/>
       <c r="D76" s="17"/>
       <c r="E76" s="17"/>
-      <c r="F76" s="138"/>
+      <c r="F76" s="139"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="125" t="s">
         <v>1309</v>
       </c>
-      <c r="B77" s="140"/>
+      <c r="B77" s="141"/>
       <c r="C77" s="119"/>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
-      <c r="F77" s="138"/>
+      <c r="F77" s="139"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="125" t="s">
         <v>1312</v>
       </c>
-      <c r="B78" s="140"/>
+      <c r="B78" s="141"/>
       <c r="C78" s="119"/>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
-      <c r="F78" s="138"/>
+      <c r="F78" s="139"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="140"/>
+      <c r="B79" s="141"/>
       <c r="C79" s="119"/>
       <c r="D79" s="17"/>
       <c r="E79" s="17"/>
@@ -20497,7 +20574,7 @@
       <c r="A80" s="17" t="s">
         <v>1317</v>
       </c>
-      <c r="B80" s="140"/>
+      <c r="B80" s="141"/>
       <c r="C80" s="119"/>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
@@ -22723,7 +22800,7 @@
       <c r="A2" s="142" t="s">
         <v>749</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="139" t="s">
         <v>430</v>
       </c>
       <c r="C2" s="52" t="s">
@@ -22744,7 +22821,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="142"/>
-      <c r="B3" s="138"/>
+      <c r="B3" s="139"/>
       <c r="C3" s="52" t="s">
         <v>432</v>
       </c>
@@ -22784,7 +22861,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="142"/>
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="139" t="s">
         <v>436</v>
       </c>
       <c r="C5" s="52" t="s">
@@ -22805,7 +22882,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="142"/>
-      <c r="B6" s="138"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="52" t="s">
         <v>750</v>
       </c>
@@ -22822,7 +22899,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="142"/>
-      <c r="B7" s="138"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="52" t="s">
         <v>735</v>
       </c>
@@ -22841,7 +22918,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="142"/>
-      <c r="B8" s="138"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="52" t="s">
         <v>738</v>
       </c>
@@ -22860,7 +22937,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="142"/>
-      <c r="B9" s="138" t="s">
+      <c r="B9" s="139" t="s">
         <v>748</v>
       </c>
       <c r="C9" s="52" t="s">
@@ -22881,7 +22958,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="142"/>
-      <c r="B10" s="138"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="55" t="s">
         <v>760</v>
       </c>
@@ -22941,10 +23018,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="139" t="s">
         <v>441</v>
       </c>
-      <c r="B13" s="138" t="s">
+      <c r="B13" s="139" t="s">
         <v>442</v>
       </c>
       <c r="C13" s="52" t="s">
@@ -22964,8 +23041,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="138"/>
-      <c r="B14" s="138"/>
+      <c r="A14" s="139"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="52" t="s">
         <v>445</v>
       </c>
@@ -22983,8 +23060,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="138"/>
-      <c r="B15" s="138"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="139"/>
       <c r="C15" s="52" t="s">
         <v>479</v>
       </c>
@@ -23000,8 +23077,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="138"/>
-      <c r="B16" s="138"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="139"/>
       <c r="C16" s="52" t="s">
         <v>746</v>
       </c>
@@ -23019,8 +23096,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="138"/>
-      <c r="B17" s="138" t="s">
+      <c r="A17" s="139"/>
+      <c r="B17" s="139" t="s">
         <v>450</v>
       </c>
       <c r="C17" s="52" t="s">
@@ -23038,8 +23115,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="138"/>
-      <c r="B18" s="138"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="139"/>
       <c r="C18" s="52" t="s">
         <v>451</v>
       </c>
@@ -23055,10 +23132,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="138" t="s">
+      <c r="A19" s="139" t="s">
         <v>452</v>
       </c>
-      <c r="B19" s="138" t="s">
+      <c r="B19" s="139" t="s">
         <v>453</v>
       </c>
       <c r="C19" s="52" t="s">
@@ -23078,8 +23155,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="138"/>
-      <c r="B20" s="138"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="139"/>
       <c r="C20" s="52" t="s">
         <v>455</v>
       </c>
@@ -23095,7 +23172,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="138"/>
+      <c r="A21" s="139"/>
       <c r="B21" s="55" t="s">
         <v>456</v>
       </c>
@@ -23116,10 +23193,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="138" t="s">
+      <c r="A22" s="139" t="s">
         <v>737</v>
       </c>
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="139" t="s">
         <v>754</v>
       </c>
       <c r="C22" s="55" t="s">
@@ -23139,8 +23216,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="138"/>
-      <c r="B23" s="138"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="139"/>
       <c r="C23" s="52" t="s">
         <v>740</v>
       </c>
@@ -23158,8 +23235,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="138"/>
-      <c r="B24" s="138"/>
+      <c r="A24" s="139"/>
+      <c r="B24" s="139"/>
       <c r="C24" s="52" t="s">
         <v>752</v>
       </c>
@@ -23177,10 +23254,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="138" t="s">
+      <c r="A25" s="139" t="s">
         <v>458</v>
       </c>
-      <c r="B25" s="138" t="s">
+      <c r="B25" s="139" t="s">
         <v>459</v>
       </c>
       <c r="C25" s="52" t="s">
@@ -23196,8 +23273,8 @@
       <c r="G25" s="55"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="138"/>
-      <c r="B26" s="138"/>
+      <c r="A26" s="139"/>
+      <c r="B26" s="139"/>
       <c r="C26" s="52" t="s">
         <v>460</v>
       </c>
@@ -23211,8 +23288,8 @@
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="138"/>
-      <c r="B27" s="138"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="52" t="s">
         <v>461</v>
       </c>
@@ -23226,8 +23303,8 @@
       <c r="G27" s="55"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="138"/>
-      <c r="B28" s="138"/>
+      <c r="A28" s="139"/>
+      <c r="B28" s="139"/>
       <c r="C28" s="52" t="s">
         <v>462</v>
       </c>
@@ -23241,8 +23318,8 @@
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="138"/>
-      <c r="B29" s="138"/>
+      <c r="A29" s="139"/>
+      <c r="B29" s="139"/>
       <c r="C29" s="52" t="s">
         <v>464</v>
       </c>
@@ -23258,7 +23335,7 @@
       <c r="G29" s="55"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="141" t="s">
+      <c r="A30" s="143" t="s">
         <v>506</v>
       </c>
       <c r="B30" s="55" t="s">
@@ -23279,7 +23356,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="141"/>
+      <c r="A31" s="143"/>
       <c r="B31" s="55" t="s">
         <v>759</v>
       </c>
@@ -23298,7 +23375,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="141"/>
+      <c r="A32" s="143"/>
       <c r="B32" s="55" t="s">
         <v>568</v>
       </c>
@@ -23319,7 +23396,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="138" t="s">
+      <c r="A33" s="139" t="s">
         <v>466</v>
       </c>
       <c r="B33" s="55" t="s">
@@ -23342,7 +23419,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="138"/>
+      <c r="A34" s="139"/>
       <c r="B34" s="55" t="s">
         <v>468</v>
       </c>
@@ -23363,10 +23440,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="138" t="s">
+      <c r="A35" s="139" t="s">
         <v>470</v>
       </c>
-      <c r="B35" s="138" t="s">
+      <c r="B35" s="139" t="s">
         <v>471</v>
       </c>
       <c r="C35" s="52" t="s">
@@ -23386,8 +23463,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="138"/>
-      <c r="B36" s="138"/>
+      <c r="A36" s="139"/>
+      <c r="B36" s="139"/>
       <c r="C36" s="52" t="s">
         <v>473</v>
       </c>
@@ -23470,7 +23547,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="138" t="s">
+      <c r="A40" s="139" t="s">
         <v>490</v>
       </c>
       <c r="B40" s="55" t="s">
@@ -23491,7 +23568,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="138"/>
+      <c r="A41" s="139"/>
       <c r="B41" s="55" t="s">
         <v>493</v>
       </c>
@@ -23510,7 +23587,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="138" t="s">
+      <c r="A42" s="139" t="s">
         <v>496</v>
       </c>
       <c r="B42" s="55" t="s">
@@ -23533,7 +23610,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="138"/>
+      <c r="A43" s="139"/>
       <c r="B43" s="55" t="s">
         <v>522</v>
       </c>
@@ -23552,7 +23629,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="138"/>
+      <c r="A44" s="139"/>
       <c r="B44" s="55" t="s">
         <v>523</v>
       </c>
@@ -23571,7 +23648,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A45" s="138"/>
+      <c r="A45" s="139"/>
       <c r="B45" s="55" t="s">
         <v>524</v>
       </c>
@@ -23590,7 +23667,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A46" s="138"/>
+      <c r="A46" s="139"/>
       <c r="B46" s="55" t="s">
         <v>525</v>
       </c>
@@ -23609,7 +23686,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A47" s="138"/>
+      <c r="A47" s="139"/>
       <c r="B47" s="55" t="s">
         <v>526</v>
       </c>
@@ -23628,7 +23705,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="138"/>
+      <c r="A48" s="139"/>
       <c r="B48" s="55" t="s">
         <v>500</v>
       </c>
@@ -23649,7 +23726,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A49" s="138"/>
+      <c r="A49" s="139"/>
       <c r="B49" s="55" t="s">
         <v>501</v>
       </c>
@@ -23690,6 +23767,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A19:A21"/>
@@ -23699,16 +23786,6 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23750,11 +23827,11 @@
       </c>
       <c r="D1" s="56"/>
       <c r="E1" s="56"/>
-      <c r="F1" s="146" t="s">
+      <c r="F1" s="147" t="s">
         <v>767</v>
       </c>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
       <c r="K1" s="70" t="s">
         <v>770</v>
       </c>
@@ -24668,16 +24745,16 @@
     <row r="26" spans="4:19" x14ac:dyDescent="0.15">
       <c r="D26"/>
       <c r="E26"/>
-      <c r="F26" s="137" t="s">
+      <c r="F26" s="138" t="s">
         <v>722</v>
       </c>
-      <c r="G26" s="137" t="s">
+      <c r="G26" s="138" t="s">
         <v>1023</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>681</v>
       </c>
-      <c r="I26" s="143" t="s">
+      <c r="I26" s="144" t="s">
         <v>763</v>
       </c>
       <c r="K26" s="69" t="s">
@@ -24700,12 +24777,12 @@
     <row r="27" spans="4:19" x14ac:dyDescent="0.15">
       <c r="D27"/>
       <c r="E27"/>
-      <c r="F27" s="137"/>
-      <c r="G27" s="137"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="138"/>
       <c r="H27" s="20" t="s">
         <v>678</v>
       </c>
-      <c r="I27" s="144"/>
+      <c r="I27" s="145"/>
       <c r="K27" s="69" t="s">
         <v>850</v>
       </c>
@@ -24726,12 +24803,12 @@
     <row r="28" spans="4:19" x14ac:dyDescent="0.15">
       <c r="D28"/>
       <c r="E28"/>
-      <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
+      <c r="F28" s="138"/>
+      <c r="G28" s="138"/>
       <c r="H28" s="20" t="s">
         <v>679</v>
       </c>
-      <c r="I28" s="145"/>
+      <c r="I28" s="146"/>
       <c r="K28" s="69" t="s">
         <v>790</v>
       </c>

</xml_diff>